<commit_message>
Setting figures and stuff
</commit_message>
<xml_diff>
--- a/data/prey_composition/Nuts_in_preys_full_corrected.xlsx
+++ b/data/prey_composition/Nuts_in_preys_full_corrected.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023\Model\data\nutrient_prey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023\Analyses\Cetacean.excretion.global\data\prey_composition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC50030-1093-4042-99FA-E1E7EA2A2A8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC745FE-EA9C-4115-A6A4-43B2A69D71C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{5321A5F6-614B-4D16-B2F5-B4F3F9C28D41}"/>
   </bookViews>
@@ -1335,9 +1335,9 @@
   <dimension ref="A1:AA155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="590" topLeftCell="A97" activePane="bottomLeft"/>
+      <pane ySplit="585" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>